<commit_message>
a couple teeny tiny edits to the dict
</commit_message>
<xml_diff>
--- a/Pew Issue Polling 2022.xlsx
+++ b/Pew Issue Polling 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93e204b33667c00b/Data Science/Milestone I/Team Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="265" documentId="13_ncr:1_{6FE855BD-3D30-4B86-9139-7CD82BFD13A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09C49B41-5208-4353-AC5F-57C496DC752D}"/>
+  <xr:revisionPtr revIDLastSave="281" documentId="13_ncr:1_{6FE855BD-3D30-4B86-9139-7CD82BFD13A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C4C2C2-79EB-4D23-B188-7004DC995491}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B322058-FDF6-4556-8742-D7743EEEB939}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>issue</t>
   </si>
   <si>
-    <t>supreme court,justices</t>
-  </si>
-  <si>
     <t>small government,big government,spending cuts,debt ceiling,government debt</t>
   </si>
   <si>
@@ -131,15 +128,9 @@
     <t>energy policy,green new deal,renewable energy,renewables,wind,solar,electrification,fossil fuels,oil,coal,nuclear power</t>
   </si>
   <si>
-    <t>crime,theft,violent,violence,homeless,rule of law,law and order,gangs</t>
-  </si>
-  <si>
     <t>abortion,anti abortion,pro choice,pro life,roe,wade,dobbs,reproductive rights,third trimester,terminate pregnancy,my body my choice</t>
   </si>
   <si>
-    <t>education,schools,school,teachers,teacher,class,classroom,classrooms,book ban,parents,school funding,learning,students</t>
-  </si>
-  <si>
     <t>health care,health insurance,uninsured,obamacare,affordable care act</t>
   </si>
   <si>
@@ -161,23 +152,32 @@
     <t>biden investigation,biden investigations,hunter biden,laptop,burisma,delaware classified documents</t>
   </si>
   <si>
-    <t>dict</t>
-  </si>
-  <si>
     <t>coronavirus,covid,pandemic,vaccine,vaccines,masks,virus,fauci,mask mandate</t>
   </si>
   <si>
     <t>future of democracy,democracy in jeopardy,january 6,january 6th,attempted coup,insurrection,seditious conspiracy,sedition,capitol riot,capitol protest</t>
   </si>
   <si>
-    <t>foreign policy,war in ukraine,donbass,crimea,war,russian invasion,china,nato,putin,xi,jinping,sanctions,taiwan,international,world leaders,north korea,european union,israel,iran,afghanistan</t>
+    <t>primary dict</t>
+  </si>
+  <si>
+    <t>crime,criminals,theft,violent crime,criminal violence,homeless,rule of law,law and order,gangs</t>
+  </si>
+  <si>
+    <t>foreign policy,war,china,nato,putin,xi,jinping,sanctions,taiwan,international,world leaders,north korea,european union,israel,iran,afghanistan</t>
+  </si>
+  <si>
+    <t>education,schools,school,teachers,teacher,classroom,classrooms,book bans,banned book,parents,school funding,students,age appropriate,sex ed</t>
+  </si>
+  <si>
+    <t>supreme court nomination,supreme court appointee,justices,appoint judges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,13 +188,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -222,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -242,21 +235,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -305,7 +283,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -628,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A001545-9124-4A37-A664-E811195959EB}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +616,7 @@
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="33" customWidth="1"/>
+    <col min="14" max="14" width="33" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -681,8 +659,8 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>40</v>
+      <c r="N1" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -725,11 +703,11 @@
       <c r="M2" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -769,8 +747,8 @@
       <c r="M3" s="3">
         <v>0</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>32</v>
+      <c r="N3" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -813,11 +791,11 @@
       <c r="M4" s="3">
         <v>1.9999999999999962E-2</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -857,8 +835,8 @@
       <c r="M5" s="3">
         <v>-1.9999999999999962E-2</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>30</v>
+      <c r="N5" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -901,8 +879,8 @@
       <c r="M6" s="3">
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>33</v>
+      <c r="N6" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -945,8 +923,8 @@
       <c r="M7" s="3">
         <v>7.999999999999996E-2</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>34</v>
+      <c r="N7" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -989,8 +967,8 @@
       <c r="M8" s="3">
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="N8" s="6" t="s">
-        <v>29</v>
+      <c r="N8" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1033,8 +1011,8 @@
       <c r="M9" s="3">
         <v>-3.0000000000000027E-2</v>
       </c>
-      <c r="N9" s="6" t="s">
-        <v>35</v>
+      <c r="N9" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="78" thickBot="1" x14ac:dyDescent="0.3">
@@ -1077,11 +1055,11 @@
       <c r="M10" s="3">
         <v>-2.0000000000000018E-2</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1121,8 +1099,8 @@
       <c r="M11" s="3">
         <v>9.9999999999999978E-2</v>
       </c>
-      <c r="N11" s="6" t="s">
-        <v>26</v>
+      <c r="N11" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1165,8 +1143,8 @@
       <c r="M12" s="3">
         <v>0</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>27</v>
+      <c r="N12" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1209,7 +1187,7 @@
       <c r="M13" s="3">
         <v>4.0000000000000036E-2</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1253,11 +1231,11 @@
       <c r="M14" s="3">
         <v>-2.0000000000000018E-2</v>
       </c>
-      <c r="N14" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="78" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -1297,8 +1275,8 @@
       <c r="M15" s="3">
         <v>-4.0000000000000036E-2</v>
       </c>
-      <c r="N15" s="6" t="s">
-        <v>43</v>
+      <c r="N15" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -1341,8 +1319,8 @@
       <c r="M16" s="3">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="N16" s="4" t="s">
-        <v>41</v>
+      <c r="N16" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="78" thickBot="1" x14ac:dyDescent="0.3">
@@ -1367,11 +1345,11 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1393,11 +1371,11 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1419,8 +1397,8 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="6" t="s">
-        <v>39</v>
+      <c r="N19" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>